<commit_message>
Remplacement des zéros des fichiers excels par des None + commentaires
</commit_message>
<xml_diff>
--- a/verif_int.xlsx
+++ b/verif_int.xlsx
@@ -115,7 +115,7 @@
     <t>Dans un endroit suffisamment éloigné du danger et de ses conséquences</t>
   </si>
   <si>
-    <t>(9, 0)</t>
+    <t>(9, None)</t>
   </si>
   <si>
     <t xml:space="preserve">VÉRIFIEZ​ ​LA​ ​PRÉSENCE​ ​DU​ ​CERTIFICAT​ ​D'IMMATRICULATION​ ​DU​ ​VÉHICULE​ ​(CARTE GRISE) </t>
@@ -133,7 +133,7 @@
     <t>Pour permettre aux services de secours d'apporter les moyens adaptés aux victimes dans le délai le plus court</t>
   </si>
   <si>
-    <t>(11, 0)</t>
+    <t>(11, None)</t>
   </si>
   <si>
     <t>MONTREZ​ ​L'INDICATEUR​ ​DE​ ​NIVEAU​ ​DE​ ​CARBURANT</t>
@@ -213,7 +213,7 @@
     <t>1. ALERTER: alerter immédiatement les secours | 2. MASSER: pratiquer une réanimation cardio-pulmonaire | 3. DÉFIBRILLER: utiliser un défibrillateur automatique (DAE) si possible</t>
   </si>
   <si>
-    <t>(19, 0)</t>
+    <t>(19, None)</t>
   </si>
   <si>
     <t xml:space="preserve">MONTREZ​ ​LA​ ​COMMANDE​ ​DE​ ​RÉGLAGE​ ​DU​ ​VOLANT </t>
@@ -252,7 +252,7 @@
 événement grave est en train de se produire</t>
   </si>
   <si>
-    <t>(23, 0)</t>
+    <t>(23, None)</t>
   </si>
   <si>
     <t>​MONTREZ​ ​LE​ ​VOYANT​ ​D'ALERTE​ ​SIGNALANT​ ​UN​ ​DÉFAUT​ ​DE​ ​BATTERIE</t>
@@ -270,7 +270,7 @@
     <t>10 ans</t>
   </si>
   <si>
-    <t>(25, 0)</t>
+    <t>(25, None)</t>
   </si>
   <si>
     <t xml:space="preserve">DE​ ​QUELLE​ ​COULEUR​ ​EST​ ​LE​ ​VOYANT​ ​QUI​ ​INDIQUE​ ​UNE​ ​DÉFAILLANCE​ ​DU​ ​SYSTÈME DE​ ​FREINAGE​ ​? </t>
@@ -306,7 +306,7 @@
     <t>Car il peut nous conseiller ou nous guider dans la réalisation des gestes à faire, ou ne pas faire, jusqu’à l’arrivée des secours</t>
   </si>
   <si>
-    <t>(29, 0)</t>
+    <t>(29, None)</t>
   </si>
   <si>
     <t>​MONTREZ​ ​LE​ ​VOYANT​ ​SIGNALANT​ ​LA​ ​MAUVAISE​ ​FERMETURE​ ​D'UNE​ ​PORTIÈRE</t>
@@ -347,7 +347,7 @@
 autorités dès que leur consultation est possible | 3. Respecter les consignes des autorités</t>
   </si>
   <si>
-    <t>(33, 0)</t>
+    <t>(33, None)</t>
   </si>
   <si>
     <t xml:space="preserve">​MONTREZ​ ​LA​ ​COMMANDE​ ​PERMETTANT​ ​D’ACTIONNER​ ​LE​ ​RÉGULATEUR​ ​DE​ ​VITESSE </t>
@@ -365,7 +365,7 @@
     <t>En indiquant le numéro de l’autoroute, le sens de circulation et le point kilométrique</t>
   </si>
   <si>
-    <t>(35, 0)</t>
+    <t>(35, None)</t>
   </si>
   <si>
     <t xml:space="preserve">SANS​ ​L'ACTIONNER,​ ​MONTREZ​ ​LA​ ​COMMANDE​ ​DE​ ​L'AVERTISSEUR​ ​SONORE </t>
@@ -417,7 +417,7 @@
     <t>Il se compose de deux codes distincts : 1. le Signal National d’Alerte (SNA) : variation du signal sur trois cycles successifs | 2. le signal de fin d’alerte : signal continu</t>
   </si>
   <si>
-    <t>(41, 0)</t>
+    <t>(41, None)</t>
   </si>
   <si>
     <t xml:space="preserve">VÉRIFIEZ​ ​LA​ ​PRÉSENCE​ ​DE​ ​L'ATTESTATION​ ​D'ASSURANCE​ ​DU​ ​VÉHICULE​ ​ET​ ​DE​ ​SA VIGNETTE​ ​SUR​ ​LE​ ​PARE-BRISE </t>
@@ -452,7 +452,7 @@
 </t>
   </si>
   <si>
-    <t>(45, 0)</t>
+    <t>(45, None)</t>
   </si>
   <si>
     <t>MONTREZ​ ​COMMENT​ ​RÉGLER​ ​LA​ ​HAUTEUR​ ​DE​ ​L'APPUI-TÊTE​ ​DU​ ​SIÈGE​ ​CONDUCTEUR</t>
@@ -470,7 +470,7 @@
     <t>L’alerte doit être donnée à l’aide d’un téléphone portable ou à défaut d’un téléphone fixe ou d’une borne d’appel d’urgence.</t>
   </si>
   <si>
-    <t>(47, 0)</t>
+    <t>(47, None)</t>
   </si>
   <si>
     <t>​DE​ ​QUELLE​ ​COULEUR​ ​EST​ ​LE​ ​VOYANT​ ​QUI​ ​INDIQUE​ ​AU​ ​CONDUCTEUR​ ​QUE​ ​LE​ ​FEU​ ​DE BROUILLARD​ ​ARRIÈRE​ ​EST​ ​ALLUMÉ​ ​?</t>
@@ -524,7 +524,7 @@
     <t>Avertir la population d’un danger imminent ou qu’un événement Grave est en train de se produire</t>
   </si>
   <si>
-    <t>(53, 0)</t>
+    <t>(53, None)</t>
   </si>
   <si>
     <t>VÉRIFIEZ​ ​LA​ ​PRÉSENCE​ ​DU​ ​CONSTAT​ ​AMIABLE​ ​DANS​ ​LE​ ​VÉHICULE</t>
@@ -542,7 +542,7 @@
     <t>La mort de la victime qui survient en quelques minutes</t>
   </si>
   <si>
-    <t>(55, 0)</t>
+    <t>(55, None)</t>
   </si>
   <si>
     <t xml:space="preserve">DE​ ​QUELLE​ ​COULEUR​ ​EST​ ​LE​ ​VOYANT​ ​QUI​ ​INDIQUE​ ​UNE​ ​DÉFAILLANCE​ ​DU​ ​SYSTÈME DE​ ​FREINAGE </t>
@@ -557,7 +557,7 @@
     <t>En appuyant fortement sur l’endroit qui saigne avec les doigts ou avec la paume de la main en mettant un tissu propre sur la plaie</t>
   </si>
   <si>
-    <t>(57, 0)</t>
+    <t>(57, None)</t>
   </si>
   <si>
     <t>SI​ ​LE​ ​VÉHICULE​ ​EN​ ​EST​ ​ÉQUIPÉ,​ ​MONTREZ​ ​LA​ ​COMMANDE​ ​DU​ ​LIMITEUR​ ​DE​ ​VITESSE</t>
@@ -590,7 +590,7 @@
     <t>1. La placer en position stable sur le côté ou position latérale de sécurité | 2. Alerter les secours | 3. Surveiller la respiration de la victime jusqu'à l'arrivée des secours</t>
   </si>
   <si>
-    <t>(61, 0)</t>
+    <t>(61, None)</t>
   </si>
   <si>
     <t>​INDIQUEZ​ ​OÙ​ ​SE​ ​SITUENT​ ​LES​ ​ATTACHES​ ​DE​ ​TYPE​ ​ISOFIX​ ​DANS​ ​LE​ ​VÉHICULE</t>
@@ -623,7 +623,7 @@
     <t>Le coeur ne fonctionne plus ou de façon anarchique</t>
   </si>
   <si>
-    <t>(81, 0)</t>
+    <t>(81, None)</t>
   </si>
   <si>
     <t>En général, en cas de panne ou d’accident, où doit être placé le triangle de présignalisation ?</t>
@@ -1065,7 +1065,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" ht="95.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>